<commit_message>
fix dob on form 1 update list
</commit_message>
<xml_diff>
--- a/public/files/students.xlsx
+++ b/public/files/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\projects\api\tranquillity\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03578E6-3C3A-4E31-AFCE-05571A502862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7875F-A451-473B-A147-4383BC01F647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="599">
   <si>
     <t>id</t>
   </si>
@@ -1271,6 +1271,567 @@
   </si>
   <si>
     <t>0545477322</t>
+  </si>
+  <si>
+    <t>2012-02-29</t>
+  </si>
+  <si>
+    <t>2013-07-16</t>
+  </si>
+  <si>
+    <t>2011-10-20</t>
+  </si>
+  <si>
+    <t>2012-11-03</t>
+  </si>
+  <si>
+    <t>2011-10-02</t>
+  </si>
+  <si>
+    <t>2012-02-02</t>
+  </si>
+  <si>
+    <t>2012-04-08</t>
+  </si>
+  <si>
+    <t>2011-12-12</t>
+  </si>
+  <si>
+    <t>2012-06-09</t>
+  </si>
+  <si>
+    <t>2011-07-03</t>
+  </si>
+  <si>
+    <t>2013-07-23</t>
+  </si>
+  <si>
+    <t>2012-06-13</t>
+  </si>
+  <si>
+    <t>2013-04-12</t>
+  </si>
+  <si>
+    <t>2012-10-15</t>
+  </si>
+  <si>
+    <t>2013-11-08</t>
+  </si>
+  <si>
+    <t>2012-09-05</t>
+  </si>
+  <si>
+    <t>2012-07-08</t>
+  </si>
+  <si>
+    <t>2012-04-24</t>
+  </si>
+  <si>
+    <t>2011-09-12</t>
+  </si>
+  <si>
+    <t>2013-08-22</t>
+  </si>
+  <si>
+    <t>2012-04-13</t>
+  </si>
+  <si>
+    <t>2012-10-27</t>
+  </si>
+  <si>
+    <t>2012-08-14</t>
+  </si>
+  <si>
+    <t>2013-05-26</t>
+  </si>
+  <si>
+    <t>2013-11-16</t>
+  </si>
+  <si>
+    <t>2011-12-04</t>
+  </si>
+  <si>
+    <t>2012-11-17</t>
+  </si>
+  <si>
+    <t>2013-02-22</t>
+  </si>
+  <si>
+    <t>2011-10-24</t>
+  </si>
+  <si>
+    <t>2013-09-08</t>
+  </si>
+  <si>
+    <t>2012-06-24</t>
+  </si>
+  <si>
+    <t>2012-04-02</t>
+  </si>
+  <si>
+    <t>2012-01-20</t>
+  </si>
+  <si>
+    <t>2012-02-12</t>
+  </si>
+  <si>
+    <t>2012-05-07</t>
+  </si>
+  <si>
+    <t>2012-01-18</t>
+  </si>
+  <si>
+    <t>2012-07-01</t>
+  </si>
+  <si>
+    <t>2011-01-07</t>
+  </si>
+  <si>
+    <t>2011-04-18</t>
+  </si>
+  <si>
+    <t>2012-01-30</t>
+  </si>
+  <si>
+    <t>2011-04-27</t>
+  </si>
+  <si>
+    <t>2011-11-29</t>
+  </si>
+  <si>
+    <t>2012-03-13</t>
+  </si>
+  <si>
+    <t>2012-03-30</t>
+  </si>
+  <si>
+    <t>2011-07-06</t>
+  </si>
+  <si>
+    <t>2011-10-17</t>
+  </si>
+  <si>
+    <t>2011-01-01</t>
+  </si>
+  <si>
+    <t>2011-01-19</t>
+  </si>
+  <si>
+    <t>2012-07-17</t>
+  </si>
+  <si>
+    <t>2011-03-11</t>
+  </si>
+  <si>
+    <t>2011-06-20</t>
+  </si>
+  <si>
+    <t>2011-11-15</t>
+  </si>
+  <si>
+    <t>2011-09-21</t>
+  </si>
+  <si>
+    <t>2012-07-28</t>
+  </si>
+  <si>
+    <t>2011-12-14</t>
+  </si>
+  <si>
+    <t>2011-12-23</t>
+  </si>
+  <si>
+    <t>2012-03-03</t>
+  </si>
+  <si>
+    <t>2012-02-23</t>
+  </si>
+  <si>
+    <t>2011-04-13</t>
+  </si>
+  <si>
+    <t>2011-08-31</t>
+  </si>
+  <si>
+    <t>2011-09-27</t>
+  </si>
+  <si>
+    <t>2011-11-24</t>
+  </si>
+  <si>
+    <t>2011-08-12</t>
+  </si>
+  <si>
+    <t>2013-01-22</t>
+  </si>
+  <si>
+    <t>2013-03-12</t>
+  </si>
+  <si>
+    <t>2012-11-22</t>
+  </si>
+  <si>
+    <t>2012-02-25</t>
+  </si>
+  <si>
+    <t>2013-08-20</t>
+  </si>
+  <si>
+    <t>2024-02-28</t>
+  </si>
+  <si>
+    <t>2011-09-26</t>
+  </si>
+  <si>
+    <t>2012-11-29</t>
+  </si>
+  <si>
+    <t>2012-07-31</t>
+  </si>
+  <si>
+    <t>2012-04-05</t>
+  </si>
+  <si>
+    <t>2013-12-25</t>
+  </si>
+  <si>
+    <t>2012-09-21</t>
+  </si>
+  <si>
+    <t>2011-10-11</t>
+  </si>
+  <si>
+    <t>2013-10-16</t>
+  </si>
+  <si>
+    <t>2011-11-23</t>
+  </si>
+  <si>
+    <t>2011-09-25</t>
+  </si>
+  <si>
+    <t>2012-02-18</t>
+  </si>
+  <si>
+    <t>2012-01-24</t>
+  </si>
+  <si>
+    <t>2012-10-13</t>
+  </si>
+  <si>
+    <t>2013-09-27</t>
+  </si>
+  <si>
+    <t>2025-05-12</t>
+  </si>
+  <si>
+    <t>2010-12-30</t>
+  </si>
+  <si>
+    <t>2013-03-07</t>
+  </si>
+  <si>
+    <t>2011-06-24</t>
+  </si>
+  <si>
+    <t>2012-07-05</t>
+  </si>
+  <si>
+    <t>2013-03-05</t>
+  </si>
+  <si>
+    <t>2013-03-20</t>
+  </si>
+  <si>
+    <t>2012-05-14</t>
+  </si>
+  <si>
+    <t>2011-12-05</t>
+  </si>
+  <si>
+    <t>2011-08-27</t>
+  </si>
+  <si>
+    <t>2011-02-11</t>
+  </si>
+  <si>
+    <t>2012-07-19</t>
+  </si>
+  <si>
+    <t>2011-04-11</t>
+  </si>
+  <si>
+    <t>2010-11-16</t>
+  </si>
+  <si>
+    <t>2013-10-12</t>
+  </si>
+  <si>
+    <t>2012-05-21</t>
+  </si>
+  <si>
+    <t>2011-09-20</t>
+  </si>
+  <si>
+    <t>2013-01-03</t>
+  </si>
+  <si>
+    <t>2013-05-07</t>
+  </si>
+  <si>
+    <t>2012-03-05</t>
+  </si>
+  <si>
+    <t>2013-05-30</t>
+  </si>
+  <si>
+    <t>2012-08-19</t>
+  </si>
+  <si>
+    <t>2013-07-17</t>
+  </si>
+  <si>
+    <t>2012-10-21</t>
+  </si>
+  <si>
+    <t>2012-05-15</t>
+  </si>
+  <si>
+    <t>2013-03-22</t>
+  </si>
+  <si>
+    <t>2011-06-08</t>
+  </si>
+  <si>
+    <t>2012-12-02</t>
+  </si>
+  <si>
+    <t>2012-03-17</t>
+  </si>
+  <si>
+    <t>2025-05-31</t>
+  </si>
+  <si>
+    <t>2012-03-02</t>
+  </si>
+  <si>
+    <t>2013-05-05</t>
+  </si>
+  <si>
+    <t>2011-10-12</t>
+  </si>
+  <si>
+    <t>2012-08-24</t>
+  </si>
+  <si>
+    <t>2012-12-06</t>
+  </si>
+  <si>
+    <t>2011-05-30</t>
+  </si>
+  <si>
+    <t>2013-02-21</t>
+  </si>
+  <si>
+    <t>2011-06-03</t>
+  </si>
+  <si>
+    <t>2011-10-21</t>
+  </si>
+  <si>
+    <t>2013-05-18</t>
+  </si>
+  <si>
+    <t>2013-10-06</t>
+  </si>
+  <si>
+    <t>2013-12-07</t>
+  </si>
+  <si>
+    <t>2012-10-17</t>
+  </si>
+  <si>
+    <t>2012-01-13</t>
+  </si>
+  <si>
+    <t>2012-02-05</t>
+  </si>
+  <si>
+    <t>2013-03-14</t>
+  </si>
+  <si>
+    <t>2012-09-04</t>
+  </si>
+  <si>
+    <t>2012-10-18</t>
+  </si>
+  <si>
+    <t>2012-07-23</t>
+  </si>
+  <si>
+    <t>2013-04-05</t>
+  </si>
+  <si>
+    <t>2012-10-23</t>
+  </si>
+  <si>
+    <t>2013-01-18</t>
+  </si>
+  <si>
+    <t>2012-06-18</t>
+  </si>
+  <si>
+    <t>2013-11-15</t>
+  </si>
+  <si>
+    <t>2012-08-22</t>
+  </si>
+  <si>
+    <t>2011-06-16</t>
+  </si>
+  <si>
+    <t>2013-03-19</t>
+  </si>
+  <si>
+    <t>2011-12-15</t>
+  </si>
+  <si>
+    <t>2012-01-02</t>
+  </si>
+  <si>
+    <t>2013-09-02</t>
+  </si>
+  <si>
+    <t>2012-04-19</t>
+  </si>
+  <si>
+    <t>2012-01-04</t>
+  </si>
+  <si>
+    <t>2012-12-14</t>
+  </si>
+  <si>
+    <t>2012-11-13</t>
+  </si>
+  <si>
+    <t>2011-09-22</t>
+  </si>
+  <si>
+    <t>2012-12-04</t>
+  </si>
+  <si>
+    <t>2012-01-03</t>
+  </si>
+  <si>
+    <t>2013-02-26</t>
+  </si>
+  <si>
+    <t>2012-02-04</t>
+  </si>
+  <si>
+    <t>2012-11-20</t>
+  </si>
+  <si>
+    <t>2013-01-09</t>
+  </si>
+  <si>
+    <t>2013-09-06</t>
+  </si>
+  <si>
+    <t>2013-03-08</t>
+  </si>
+  <si>
+    <t>2012-02-17</t>
+  </si>
+  <si>
+    <t>2011-12-10</t>
+  </si>
+  <si>
+    <t>2012-01-12</t>
+  </si>
+  <si>
+    <t>2013-11-03</t>
+  </si>
+  <si>
+    <t>2012-06-04</t>
+  </si>
+  <si>
+    <t>2013-02-17</t>
+  </si>
+  <si>
+    <t>2012-05-27</t>
+  </si>
+  <si>
+    <t>2012-04-01</t>
+  </si>
+  <si>
+    <t>2012-08-11</t>
+  </si>
+  <si>
+    <t>2012-08-12</t>
+  </si>
+  <si>
+    <t>2011-10-27</t>
+  </si>
+  <si>
+    <t>2013-06-10</t>
+  </si>
+  <si>
+    <t>2012-04-10</t>
+  </si>
+  <si>
+    <t>2012-09-28</t>
+  </si>
+  <si>
+    <t>2012-01-25</t>
+  </si>
+  <si>
+    <t>2012-05-31</t>
+  </si>
+  <si>
+    <t>2012-08-05</t>
+  </si>
+  <si>
+    <t>2012-10-29</t>
+  </si>
+  <si>
+    <t>2013-02-14</t>
+  </si>
+  <si>
+    <t>2013-04-04</t>
+  </si>
+  <si>
+    <t>2013-11-02</t>
+  </si>
+  <si>
+    <t>2012-10-01</t>
+  </si>
+  <si>
+    <t>2013-11-06</t>
+  </si>
+  <si>
+    <t>2013-04-09</t>
+  </si>
+  <si>
+    <t>2013-09-04</t>
+  </si>
+  <si>
+    <t>2011-09-14</t>
+  </si>
+  <si>
+    <t>2011-11-09</t>
+  </si>
+  <si>
+    <t>2012-02-09</t>
+  </si>
+  <si>
+    <t>2011-01-24</t>
+  </si>
+  <si>
+    <t>2011-09-01</t>
+  </si>
+  <si>
+    <t>2013-12-12</t>
   </si>
 </sst>
 </file>
@@ -1608,9 +2169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A205"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,8 +2233,8 @@
       <c r="F2" s="4">
         <v>5844406822</v>
       </c>
-      <c r="G2" s="5">
-        <v>40968</v>
+      <c r="G2" s="5" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1695,8 +2256,8 @@
       <c r="F3" s="4">
         <v>7354578523</v>
       </c>
-      <c r="G3" s="5">
-        <v>41471</v>
+      <c r="G3" s="5" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1718,8 +2279,8 @@
       <c r="F4" s="4">
         <v>6820203420</v>
       </c>
-      <c r="G4" s="5">
-        <v>40836</v>
+      <c r="G4" s="5" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,8 +2302,8 @@
       <c r="F5" s="4">
         <v>8053518883</v>
       </c>
-      <c r="G5" s="5">
-        <v>41216</v>
+      <c r="G5" s="5" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1764,8 +2325,8 @@
       <c r="F6" s="4">
         <v>6962657394</v>
       </c>
-      <c r="G6" s="5">
-        <v>40818</v>
+      <c r="G6" s="5" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1787,8 +2348,8 @@
       <c r="F7" s="4">
         <v>5837305561</v>
       </c>
-      <c r="G7" s="5">
-        <v>40941</v>
+      <c r="G7" s="5" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1810,8 +2371,8 @@
       <c r="F8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="5">
-        <v>41007</v>
+      <c r="G8" s="5" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1833,8 +2394,8 @@
       <c r="F9" s="4">
         <v>2731305971</v>
       </c>
-      <c r="G9" s="5">
-        <v>40889</v>
+      <c r="G9" s="5" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1856,8 +2417,8 @@
       <c r="F10" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G10" s="5">
-        <v>41069</v>
+      <c r="G10" s="5" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1879,8 +2440,8 @@
       <c r="F11" s="4">
         <v>4850516963</v>
       </c>
-      <c r="G11" s="5">
-        <v>40727</v>
+      <c r="G11" s="5" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1902,8 +2463,8 @@
       <c r="F12" s="4">
         <v>7546417212</v>
       </c>
-      <c r="G12" s="5">
-        <v>41478</v>
+      <c r="G12" s="5" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1925,8 +2486,8 @@
       <c r="F13" s="4">
         <v>7953547463</v>
       </c>
-      <c r="G13" s="5">
-        <v>41073</v>
+      <c r="G13" s="5" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,8 +2509,8 @@
       <c r="F14" s="4">
         <v>1233306911</v>
       </c>
-      <c r="G14" s="5">
-        <v>41376</v>
+      <c r="G14" s="5" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1971,8 +2532,8 @@
       <c r="F15" s="4">
         <v>1946447702</v>
       </c>
-      <c r="G15" s="5">
-        <v>41197</v>
+      <c r="G15" s="5" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1994,8 +2555,8 @@
       <c r="F16" s="4">
         <v>7632306101</v>
       </c>
-      <c r="G16" s="5">
-        <v>41586</v>
+      <c r="G16" s="5" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2017,8 +2578,8 @@
       <c r="F17" s="4">
         <v>5145466732</v>
       </c>
-      <c r="G17" s="5">
-        <v>41157</v>
+      <c r="G17" s="5" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2040,8 +2601,8 @@
       <c r="F18" s="4">
         <v>4458507343</v>
       </c>
-      <c r="G18" s="5">
-        <v>41098</v>
+      <c r="G18" s="5" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2063,8 +2624,8 @@
       <c r="F19" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="5">
-        <v>41023</v>
+      <c r="G19" s="5" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2086,8 +2647,8 @@
       <c r="F20" s="4">
         <v>9251566283</v>
       </c>
-      <c r="G20" s="5">
-        <v>40798</v>
+      <c r="G20" s="5" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2109,8 +2670,8 @@
       <c r="F21" s="4">
         <v>6022295800</v>
       </c>
-      <c r="G21" s="5">
-        <v>41508</v>
+      <c r="G21" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2132,8 +2693,8 @@
       <c r="F22" s="4">
         <v>2143456062</v>
       </c>
-      <c r="G22" s="5">
-        <v>41012</v>
+      <c r="G22" s="5" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2155,8 +2716,8 @@
       <c r="F23" s="4">
         <v>6260688354</v>
       </c>
-      <c r="G23" s="5">
-        <v>41209</v>
+      <c r="G23" s="5" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2178,8 +2739,8 @@
       <c r="F24" s="4">
         <v>5038395901</v>
       </c>
-      <c r="G24" s="5">
-        <v>41135</v>
+      <c r="G24" s="5" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2201,8 +2762,8 @@
       <c r="F25" s="4">
         <v>4038336791</v>
       </c>
-      <c r="G25" s="5">
-        <v>41420</v>
+      <c r="G25" s="5" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2224,8 +2785,8 @@
       <c r="F26" s="4">
         <v>1036376431</v>
       </c>
-      <c r="G26" s="5">
-        <v>41594</v>
+      <c r="G26" s="5" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2247,8 +2808,8 @@
       <c r="F27" s="4">
         <v>8252527093</v>
       </c>
-      <c r="G27" s="5">
-        <v>40881</v>
+      <c r="G27" s="5" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,8 +2831,8 @@
       <c r="F28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G28" s="5">
-        <v>41230</v>
+      <c r="G28" s="5" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2293,8 +2854,8 @@
       <c r="F29" s="4">
         <v>2147417562</v>
       </c>
-      <c r="G29" s="5">
-        <v>41327</v>
+      <c r="G29" s="5" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2316,8 +2877,8 @@
       <c r="F30" s="4">
         <v>2023243100</v>
       </c>
-      <c r="G30" s="5">
-        <v>40840</v>
+      <c r="G30" s="5" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2339,8 +2900,8 @@
       <c r="F31" s="4">
         <v>6864639084</v>
       </c>
-      <c r="G31" s="5">
-        <v>41525</v>
+      <c r="G31" s="5" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2362,8 +2923,8 @@
       <c r="F32" s="4">
         <v>1861648414</v>
       </c>
-      <c r="G32" s="5">
-        <v>41084</v>
+      <c r="G32" s="5" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2385,8 +2946,8 @@
       <c r="F33" s="4">
         <v>9338335941</v>
       </c>
-      <c r="G33" s="5">
-        <v>41001</v>
+      <c r="G33" s="5" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2445,8 +3006,8 @@
       <c r="F36" s="4">
         <v>9648496002</v>
       </c>
-      <c r="G36" s="5">
-        <v>40928</v>
+      <c r="G36" s="5" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2468,8 +3029,8 @@
       <c r="F37" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G37" s="5">
-        <v>40951</v>
+      <c r="G37" s="5" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2491,8 +3052,8 @@
       <c r="F38" s="4">
         <v>3123244770</v>
       </c>
-      <c r="G38" s="5">
-        <v>41036</v>
+      <c r="G38" s="5" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2514,8 +3075,8 @@
       <c r="F39" s="4">
         <v>9125224850</v>
       </c>
-      <c r="G39" s="5">
-        <v>40926</v>
+      <c r="G39" s="5" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2537,8 +3098,8 @@
       <c r="F40" s="4">
         <v>3462628084</v>
       </c>
-      <c r="G40" s="5">
-        <v>41091</v>
+      <c r="G40" s="5" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2560,8 +3121,8 @@
       <c r="F41" s="4">
         <v>2669677874</v>
       </c>
-      <c r="G41" s="5">
-        <v>40550</v>
+      <c r="G41" s="5" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2583,8 +3144,8 @@
       <c r="F42" s="4">
         <v>4126283880</v>
       </c>
-      <c r="G42" s="5">
-        <v>40651</v>
+      <c r="G42" s="5" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2606,8 +3167,8 @@
       <c r="F43" s="4">
         <v>3737385881</v>
       </c>
-      <c r="G43" s="5">
-        <v>40938</v>
+      <c r="G43" s="5" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2629,8 +3190,8 @@
       <c r="F44" s="4">
         <v>7848435242</v>
       </c>
-      <c r="G44" s="5">
-        <v>40660</v>
+      <c r="G44" s="5" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2652,8 +3213,8 @@
       <c r="F45" s="4">
         <v>8030375561</v>
       </c>
-      <c r="G45" s="5">
-        <v>40876</v>
+      <c r="G45" s="5" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2675,8 +3236,8 @@
       <c r="F46" s="4">
         <v>8135305021</v>
       </c>
-      <c r="G46" s="5">
-        <v>40981</v>
+      <c r="G46" s="5" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2698,8 +3259,8 @@
       <c r="F47" s="4">
         <v>3547426462</v>
       </c>
-      <c r="G47" s="5">
-        <v>40998</v>
+      <c r="G47" s="5" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2721,8 +3282,8 @@
       <c r="F48" s="4">
         <v>4246435522</v>
       </c>
-      <c r="G48" s="5">
-        <v>40730</v>
+      <c r="G48" s="5" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2744,8 +3305,8 @@
       <c r="F49" s="4">
         <v>4221264020</v>
       </c>
-      <c r="G49" s="5">
-        <v>40833</v>
+      <c r="G49" s="5" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2767,8 +3328,8 @@
       <c r="F50" s="4">
         <v>8459576463</v>
       </c>
-      <c r="G50" s="5">
-        <v>40544</v>
+      <c r="G50" s="5" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2790,8 +3351,8 @@
       <c r="F51" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G51" s="5">
-        <v>40562</v>
+      <c r="G51" s="5" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2813,8 +3374,8 @@
       <c r="F52" s="4">
         <v>7333345771</v>
       </c>
-      <c r="G52" s="5">
-        <v>41107</v>
+      <c r="G52" s="5" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2836,8 +3397,8 @@
       <c r="F53" s="4">
         <v>4758596643</v>
       </c>
-      <c r="G53" s="5">
-        <v>40613</v>
+      <c r="G53" s="5" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2859,8 +3420,8 @@
       <c r="F54" s="4">
         <v>5159586143</v>
       </c>
-      <c r="G54" s="5">
-        <v>40714</v>
+      <c r="G54" s="5" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2882,8 +3443,8 @@
       <c r="F55" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G55" s="5">
-        <v>40862</v>
+      <c r="G55" s="5" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2905,8 +3466,8 @@
       <c r="F56" s="4">
         <v>2652546863</v>
       </c>
-      <c r="G56" s="5">
-        <v>40807</v>
+      <c r="G56" s="5" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2928,8 +3489,8 @@
       <c r="F57" s="4">
         <v>3260658594</v>
       </c>
-      <c r="G57" s="5">
-        <v>41118</v>
+      <c r="G57" s="5" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2951,8 +3512,8 @@
       <c r="F58" s="4">
         <v>4450537023</v>
       </c>
-      <c r="G58" s="5">
-        <v>40891</v>
+      <c r="G58" s="5" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2974,8 +3535,8 @@
       <c r="F59" s="4">
         <v>3952507723</v>
       </c>
-      <c r="G59" s="5">
-        <v>40900</v>
+      <c r="G59" s="5" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2997,8 +3558,8 @@
       <c r="F60" s="4">
         <v>2422264830</v>
       </c>
-      <c r="G60" s="5">
-        <v>40971</v>
+      <c r="G60" s="5" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3020,8 +3581,8 @@
       <c r="F61" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G61" s="5">
-        <v>40962</v>
+      <c r="G61" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3043,8 +3604,8 @@
       <c r="F62" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="G62" s="5">
-        <v>40646</v>
+      <c r="G62" s="5" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3066,8 +3627,8 @@
       <c r="F63" s="4">
         <v>5850586523</v>
       </c>
-      <c r="G63" s="5">
-        <v>40786</v>
+      <c r="G63" s="5" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3089,8 +3650,8 @@
       <c r="F64" s="4">
         <v>1161647704</v>
       </c>
-      <c r="G64" s="5">
-        <v>40813</v>
+      <c r="G64" s="5" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3112,8 +3673,8 @@
       <c r="F65" s="4">
         <v>7040475672</v>
       </c>
-      <c r="G65" s="5">
-        <v>40871</v>
+      <c r="G65" s="5" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3135,8 +3696,8 @@
       <c r="F66" s="4">
         <v>7707227800</v>
       </c>
-      <c r="G66" s="5">
-        <v>40767</v>
+      <c r="G66" s="5" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3158,8 +3719,8 @@
       <c r="F67" s="4">
         <v>5849601764</v>
       </c>
-      <c r="G67" s="5">
-        <v>41296</v>
+      <c r="G67" s="5" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3181,8 +3742,8 @@
       <c r="F68" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="G68" s="5">
-        <v>41345</v>
+      <c r="G68" s="5" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3204,8 +3765,8 @@
       <c r="F69" s="4">
         <v>2430396241</v>
       </c>
-      <c r="G69" s="5">
-        <v>41235</v>
+      <c r="G69" s="5" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3227,8 +3788,8 @@
       <c r="F70" s="4">
         <v>6247496212</v>
       </c>
-      <c r="G70" s="5">
-        <v>40964</v>
+      <c r="G70" s="5" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3250,8 +3811,8 @@
       <c r="F71" s="4">
         <v>4024265420</v>
       </c>
-      <c r="G71" s="5">
-        <v>41506</v>
+      <c r="G71" s="5" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3273,8 +3834,8 @@
       <c r="F72" s="4">
         <v>9247457222</v>
       </c>
-      <c r="G72" s="5">
-        <v>45350</v>
+      <c r="G72" s="5" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3296,8 +3857,8 @@
       <c r="F73" s="4">
         <v>8339314731</v>
       </c>
-      <c r="G73" s="5">
-        <v>40876</v>
+      <c r="G73" s="5" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3319,8 +3880,8 @@
       <c r="F74" s="4">
         <v>1155528903</v>
       </c>
-      <c r="G74" s="5">
-        <v>40812</v>
+      <c r="G74" s="5" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3342,8 +3903,8 @@
       <c r="F75" s="4">
         <v>6968699664</v>
       </c>
-      <c r="G75" s="5">
-        <v>41242</v>
+      <c r="G75" s="5" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3365,8 +3926,8 @@
       <c r="F76" s="4">
         <v>3034395871</v>
       </c>
-      <c r="G76" s="5">
-        <v>41121</v>
+      <c r="G76" s="5" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3388,8 +3949,8 @@
       <c r="F77" s="4">
         <v>8930385651</v>
       </c>
-      <c r="G77" s="5">
-        <v>41004</v>
+      <c r="G77" s="5" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3411,8 +3972,8 @@
       <c r="F78" s="4">
         <v>1756579933</v>
       </c>
-      <c r="G78" s="5">
-        <v>41633</v>
+      <c r="G78" s="5" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3434,8 +3995,8 @@
       <c r="F79" s="4">
         <v>4456567713</v>
       </c>
-      <c r="G79" s="5">
-        <v>41173</v>
+      <c r="G79" s="5" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3457,8 +4018,8 @@
       <c r="F80" s="4">
         <v>5461687154</v>
       </c>
-      <c r="G80" s="5">
-        <v>40827</v>
+      <c r="G80" s="5" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3480,8 +4041,8 @@
       <c r="F81" s="4">
         <v>7361630694</v>
       </c>
-      <c r="G81" s="5">
-        <v>41563</v>
+      <c r="G81" s="5" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3503,8 +4064,8 @@
       <c r="F82" s="4">
         <v>2464648554</v>
       </c>
-      <c r="G82" s="5">
-        <v>40870</v>
+      <c r="G82" s="5" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3526,8 +4087,8 @@
       <c r="F83" s="4">
         <v>9062647044</v>
       </c>
-      <c r="G83" s="5">
-        <v>40811</v>
+      <c r="G83" s="5" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3549,8 +4110,8 @@
       <c r="F84" s="4">
         <v>8758537113</v>
       </c>
-      <c r="G84" s="5">
-        <v>40957</v>
+      <c r="G84" s="5" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3572,8 +4133,8 @@
       <c r="F85" s="4">
         <v>7943456992</v>
       </c>
-      <c r="G85" s="5">
-        <v>40932</v>
+      <c r="G85" s="5" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3595,8 +4156,8 @@
       <c r="F86" s="4">
         <v>1741406352</v>
       </c>
-      <c r="G86" s="5">
-        <v>41195</v>
+      <c r="G86" s="5" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3618,8 +4179,8 @@
       <c r="F87" s="4">
         <v>6427275830</v>
       </c>
-      <c r="G87" s="5">
-        <v>41544</v>
+      <c r="G87" s="5" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3641,8 +4202,8 @@
       <c r="F88" s="4">
         <v>4643487562</v>
       </c>
-      <c r="G88" s="5">
-        <v>45789</v>
+      <c r="G88" s="5" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3664,8 +4225,8 @@
       <c r="F89" s="4">
         <v>8825243000</v>
       </c>
-      <c r="G89" s="5">
-        <v>40542</v>
+      <c r="G89" s="5" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3687,8 +4248,8 @@
       <c r="F90" s="4">
         <v>6521295860</v>
       </c>
-      <c r="G90" s="5">
-        <v>41340</v>
+      <c r="G90" s="5" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3710,8 +4271,8 @@
       <c r="F91" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="G91" s="5">
-        <v>40718</v>
+      <c r="G91" s="5" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3733,8 +4294,8 @@
       <c r="F92" s="4">
         <v>4749406432</v>
       </c>
-      <c r="G92" s="5">
-        <v>41095</v>
+      <c r="G92" s="5" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3756,8 +4317,8 @@
       <c r="F93" s="4">
         <v>1841477822</v>
       </c>
-      <c r="G93" s="5">
-        <v>41338</v>
+      <c r="G93" s="5" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3779,8 +4340,8 @@
       <c r="F94" s="4">
         <v>1922265930</v>
       </c>
-      <c r="G94" s="5">
-        <v>41353</v>
+      <c r="G94" s="5" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3802,8 +4363,8 @@
       <c r="F95" s="4">
         <v>4926214410</v>
       </c>
-      <c r="G95" s="5">
-        <v>41043</v>
+      <c r="G95" s="5" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3825,8 +4386,8 @@
       <c r="F96" s="4">
         <v>6565688644</v>
       </c>
-      <c r="G96" s="5">
-        <v>40882</v>
+      <c r="G96" s="5" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3848,8 +4409,8 @@
       <c r="F97" s="4">
         <v>4956536743</v>
       </c>
-      <c r="G97" s="5">
-        <v>40807</v>
+      <c r="G97" s="5" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3871,8 +4432,8 @@
       <c r="F98" s="4">
         <v>9958536363</v>
       </c>
-      <c r="G98" s="5">
-        <v>40782</v>
+      <c r="G98" s="5" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3928,8 +4489,8 @@
       <c r="F101" s="4">
         <v>8745405112</v>
       </c>
-      <c r="G101" s="5">
-        <v>40585</v>
+      <c r="G101" s="5" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3951,8 +4512,8 @@
       <c r="F102" s="4">
         <v>5760668514</v>
       </c>
-      <c r="G102" s="5">
-        <v>41109</v>
+      <c r="G102" s="5" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3974,8 +4535,8 @@
       <c r="F103" s="4">
         <v>5960687254</v>
       </c>
-      <c r="G103" s="5">
-        <v>40644</v>
+      <c r="G103" s="5" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3997,8 +4558,8 @@
       <c r="F104" s="4">
         <v>3243435742</v>
       </c>
-      <c r="G104" s="5">
-        <v>40498</v>
+      <c r="G104" s="5" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4020,8 +4581,8 @@
       <c r="F105" s="4">
         <v>1528256970</v>
       </c>
-      <c r="G105" s="5">
-        <v>41559</v>
+      <c r="G105" s="5" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4043,8 +4604,8 @@
       <c r="F106" s="4">
         <v>4723264140</v>
       </c>
-      <c r="G106" s="5">
-        <v>41050</v>
+      <c r="G106" s="5" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4066,8 +4627,8 @@
       <c r="F107" s="4">
         <v>6139334841</v>
       </c>
-      <c r="G107" s="5">
-        <v>40806</v>
+      <c r="G107" s="5" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4089,8 +4650,8 @@
       <c r="F108" s="4">
         <v>2760679124</v>
       </c>
-      <c r="G108" s="5">
-        <v>41277</v>
+      <c r="G108" s="5" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4112,8 +4673,8 @@
       <c r="F109" s="4">
         <v>2544487622</v>
       </c>
-      <c r="G109" s="5">
-        <v>41401</v>
+      <c r="G109" s="5" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4135,8 +4696,8 @@
       <c r="F110" s="4">
         <v>9850547983</v>
       </c>
-      <c r="G110" s="5">
-        <v>40973</v>
+      <c r="G110" s="5" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4158,8 +4719,8 @@
       <c r="F111" s="4">
         <v>5463689134</v>
       </c>
-      <c r="G111" s="5">
-        <v>41424</v>
+      <c r="G111" s="5" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4181,8 +4742,8 @@
       <c r="F112" s="4">
         <v>2545446382</v>
       </c>
-      <c r="G112" s="5">
-        <v>41140</v>
+      <c r="G112" s="5" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4204,8 +4765,8 @@
       <c r="F113" s="4">
         <v>6043437232</v>
       </c>
-      <c r="G113" s="5">
-        <v>41472</v>
+      <c r="G113" s="5" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4227,8 +4788,8 @@
       <c r="F114" s="4">
         <v>7233345371</v>
       </c>
-      <c r="G114" s="5">
-        <v>41203</v>
+      <c r="G114" s="5" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4250,8 +4811,8 @@
       <c r="F115" s="4">
         <v>9144456442</v>
       </c>
-      <c r="G115" s="5">
-        <v>41044</v>
+      <c r="G115" s="5" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4273,8 +4834,8 @@
       <c r="F116" s="4">
         <v>7736384301</v>
       </c>
-      <c r="G116" s="5">
-        <v>40542</v>
+      <c r="G116" s="5" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4296,8 +4857,8 @@
       <c r="F117" s="4">
         <v>5037366531</v>
       </c>
-      <c r="G117" s="5">
-        <v>41355</v>
+      <c r="G117" s="5" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4319,8 +4880,8 @@
       <c r="F118" s="4">
         <v>4228273860</v>
       </c>
-      <c r="G118" s="5">
-        <v>40702</v>
+      <c r="G118" s="5" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4342,8 +4903,8 @@
       <c r="F119" s="4">
         <v>6157558813</v>
       </c>
-      <c r="G119" s="5">
-        <v>41245</v>
+      <c r="G119" s="5" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4365,8 +4926,8 @@
       <c r="F120" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G120" s="5">
-        <v>40985</v>
+      <c r="G120" s="5" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4388,8 +4949,8 @@
       <c r="F121" s="4">
         <v>4136376581</v>
       </c>
-      <c r="G121" s="5">
-        <v>41478</v>
+      <c r="G121" s="5" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4411,8 +4972,8 @@
       <c r="F122" s="4">
         <v>8338325411</v>
       </c>
-      <c r="G122" s="5">
-        <v>45808</v>
+      <c r="G122" s="5" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4434,8 +4995,8 @@
       <c r="F123" s="4">
         <v>5943406142</v>
       </c>
-      <c r="G123" s="5">
-        <v>40970</v>
+      <c r="G123" s="5" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4457,8 +5018,8 @@
       <c r="F124" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="G124" s="5">
-        <v>41399</v>
+      <c r="G124" s="5" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4480,8 +5041,8 @@
       <c r="F125" s="4">
         <v>4231394911</v>
       </c>
-      <c r="G125" s="5">
-        <v>40828</v>
+      <c r="G125" s="5" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4503,8 +5064,8 @@
       <c r="F126" s="4">
         <v>5663648974</v>
       </c>
-      <c r="G126" s="5">
-        <v>41145</v>
+      <c r="G126" s="5" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4526,8 +5087,8 @@
       <c r="F127" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G127" s="5">
-        <v>41249</v>
+      <c r="G127" s="5" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4549,8 +5110,8 @@
       <c r="F128" s="4">
         <v>6329253070</v>
       </c>
-      <c r="G128" s="5">
-        <v>40693</v>
+      <c r="G128" s="5" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4572,8 +5133,8 @@
       <c r="F129" s="4">
         <v>5052508923</v>
       </c>
-      <c r="G129" s="5">
-        <v>41326</v>
+      <c r="G129" s="5" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4595,8 +5156,8 @@
       <c r="F130" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="G130" s="5">
-        <v>40697</v>
+      <c r="G130" s="5" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4618,8 +5179,8 @@
       <c r="F131" s="4">
         <v>8541495272</v>
       </c>
-      <c r="G131" s="5">
-        <v>40837</v>
+      <c r="G131" s="5" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4641,8 +5202,8 @@
       <c r="F132" s="4">
         <v>1430336851</v>
       </c>
-      <c r="G132" s="5">
-        <v>41412</v>
+      <c r="G132" s="5" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4678,8 +5239,8 @@
       <c r="F134" s="4">
         <v>5850588163</v>
       </c>
-      <c r="G134" s="5">
-        <v>41553</v>
+      <c r="G134" s="5" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4701,8 +5262,8 @@
       <c r="F135" s="4">
         <v>3225266810</v>
       </c>
-      <c r="G135" s="5">
-        <v>41615</v>
+      <c r="G135" s="5" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4724,8 +5285,8 @@
       <c r="F136" s="4">
         <v>8551508773</v>
       </c>
-      <c r="G136" s="5">
-        <v>41199</v>
+      <c r="G136" s="5" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4747,8 +5308,8 @@
       <c r="F137" s="4">
         <v>4054517363</v>
       </c>
-      <c r="G137" s="5">
-        <v>40921</v>
+      <c r="G137" s="5" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4770,8 +5331,8 @@
       <c r="F138" s="4">
         <v>2926294090</v>
       </c>
-      <c r="G138" s="5">
-        <v>40944</v>
+      <c r="G138" s="5" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4793,8 +5354,8 @@
       <c r="F139" s="4">
         <v>282285690</v>
       </c>
-      <c r="G139" s="5">
-        <v>41347</v>
+      <c r="G139" s="5" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4816,8 +5377,8 @@
       <c r="F140" s="4">
         <v>9235375261</v>
       </c>
-      <c r="G140" s="5">
-        <v>41156</v>
+      <c r="G140" s="5" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4839,8 +5400,8 @@
       <c r="F141" s="4">
         <v>8444486532</v>
       </c>
-      <c r="G141" s="5">
-        <v>41200</v>
+      <c r="G141" s="5" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4862,8 +5423,8 @@
       <c r="F142" s="4">
         <v>4238385361</v>
       </c>
-      <c r="G142" s="5">
-        <v>40928</v>
+      <c r="G142" s="5" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4885,8 +5446,8 @@
       <c r="F143" s="4">
         <v>4824234380</v>
       </c>
-      <c r="G143" s="5">
-        <v>41113</v>
+      <c r="G143" s="5" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4908,8 +5469,8 @@
       <c r="F144" s="4">
         <v>4541447262</v>
       </c>
-      <c r="G144" s="5">
-        <v>41369</v>
+      <c r="G144" s="5" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -4931,8 +5492,8 @@
       <c r="F145" s="4">
         <v>9630325401</v>
       </c>
-      <c r="G145" s="5">
-        <v>41205</v>
+      <c r="G145" s="5" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4954,8 +5515,8 @@
       <c r="F146" s="4">
         <v>2743437522</v>
       </c>
-      <c r="G146" s="5">
-        <v>41292</v>
+      <c r="G146" s="5" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -4977,8 +5538,8 @@
       <c r="F147" s="4">
         <v>7537356111</v>
       </c>
-      <c r="G147" s="5">
-        <v>41078</v>
+      <c r="G147" s="5" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -5000,8 +5561,8 @@
       <c r="F148" s="4">
         <v>2525245220</v>
       </c>
-      <c r="G148" s="5">
-        <v>41593</v>
+      <c r="G148" s="5" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -5023,8 +5584,8 @@
       <c r="F149" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="G149" s="5">
-        <v>41143</v>
+      <c r="G149" s="5" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -5046,8 +5607,8 @@
       <c r="F150" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="G150" s="5">
-        <v>40710</v>
+      <c r="G150" s="5" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5069,8 +5630,8 @@
       <c r="F151" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="G151" s="5">
-        <v>41352</v>
+      <c r="G151" s="5" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5092,8 +5653,8 @@
       <c r="F152" s="4">
         <v>5068618374</v>
       </c>
-      <c r="G152" s="5">
-        <v>40892</v>
+      <c r="G152" s="5" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5115,8 +5676,8 @@
       <c r="F153" s="4">
         <v>5943476352</v>
       </c>
-      <c r="G153" s="5">
-        <v>40910</v>
+      <c r="G153" s="5" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5138,8 +5699,8 @@
       <c r="F154" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="G154" s="5">
-        <v>41519</v>
+      <c r="G154" s="5" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -5161,8 +5722,8 @@
       <c r="F155" s="4">
         <v>6429283170</v>
       </c>
-      <c r="G155" s="5">
-        <v>40806</v>
+      <c r="G155" s="5" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5184,8 +5745,8 @@
       <c r="F156" s="4">
         <v>3564628784</v>
       </c>
-      <c r="G156" s="5">
-        <v>41023</v>
+      <c r="G156" s="5" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5207,8 +5768,8 @@
       <c r="F157" s="4">
         <v>3550517223</v>
       </c>
-      <c r="G157" s="5">
-        <v>41018</v>
+      <c r="G157" s="5" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5230,8 +5791,8 @@
       <c r="F158" s="4">
         <v>8423244060</v>
       </c>
-      <c r="G158" s="5">
-        <v>40912</v>
+      <c r="G158" s="5" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5253,8 +5814,8 @@
       <c r="F159" s="4">
         <v>3665619364</v>
       </c>
-      <c r="G159" s="5">
-        <v>41257</v>
+      <c r="G159" s="5" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5276,8 +5837,8 @@
       <c r="F160" s="4">
         <v>2233305901</v>
       </c>
-      <c r="G160" s="5">
-        <v>41226</v>
+      <c r="G160" s="5" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5299,8 +5860,8 @@
       <c r="F161" s="4">
         <v>4557576783</v>
       </c>
-      <c r="G161" s="5">
-        <v>40808</v>
+      <c r="G161" s="5" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5322,8 +5883,8 @@
       <c r="F162" s="4">
         <v>4349487262</v>
       </c>
-      <c r="G162" s="5">
-        <v>41247</v>
+      <c r="G162" s="5" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5345,8 +5906,8 @@
       <c r="F163" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="G163" s="5">
-        <v>40911</v>
+      <c r="G163" s="5" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5368,8 +5929,8 @@
       <c r="F164" s="4">
         <v>6960628204</v>
       </c>
-      <c r="G164" s="5">
-        <v>40944</v>
+      <c r="G164" s="5" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5391,8 +5952,8 @@
       <c r="F165" s="4">
         <v>2330326041</v>
       </c>
-      <c r="G165" s="5">
-        <v>41331</v>
+      <c r="G165" s="5" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5414,8 +5975,8 @@
       <c r="F166" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="G166" s="5">
-        <v>40943</v>
+      <c r="G166" s="5" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5437,8 +5998,8 @@
       <c r="F167" s="4">
         <v>7624255260</v>
       </c>
-      <c r="G167" s="5">
-        <v>41233</v>
+      <c r="G167" s="5" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5460,8 +6021,8 @@
       <c r="F168" s="4">
         <v>7956598113</v>
       </c>
-      <c r="G168" s="5">
-        <v>41283</v>
+      <c r="G168" s="5" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -5483,8 +6044,8 @@
       <c r="F169" s="4">
         <v>6345447772</v>
       </c>
-      <c r="G169" s="5">
-        <v>41523</v>
+      <c r="G169" s="5" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -5506,8 +6067,8 @@
       <c r="F170" s="4">
         <v>5657548473</v>
       </c>
-      <c r="G170" s="5">
-        <v>41341</v>
+      <c r="G170" s="5" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -5529,8 +6090,8 @@
       <c r="F171" s="4">
         <v>4851517633</v>
       </c>
-      <c r="G171" s="5">
-        <v>40956</v>
+      <c r="G171" s="5" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -5552,8 +6113,8 @@
       <c r="F172" s="4">
         <v>9135365911</v>
       </c>
-      <c r="G172" s="5">
-        <v>40887</v>
+      <c r="G172" s="5" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5575,8 +6136,8 @@
       <c r="F173" s="4">
         <v>9147456822</v>
       </c>
-      <c r="G173" s="5">
-        <v>40920</v>
+      <c r="G173" s="5" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -5598,8 +6159,8 @@
       <c r="F174" s="4">
         <v>9356577533</v>
       </c>
-      <c r="G174" s="5">
-        <v>41073</v>
+      <c r="G174" s="5" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5621,8 +6182,8 @@
       <c r="F175" s="4">
         <v>7335327401</v>
       </c>
-      <c r="G175" s="5">
-        <v>41581</v>
+      <c r="G175" s="5" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5644,8 +6205,8 @@
       <c r="F176" s="4">
         <v>7967668004</v>
       </c>
-      <c r="G176" s="5">
-        <v>41064</v>
+      <c r="G176" s="5" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5667,8 +6228,8 @@
       <c r="F177" s="4">
         <v>2525275600</v>
       </c>
-      <c r="G177" s="5">
-        <v>41322</v>
+      <c r="G177" s="5" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5690,8 +6251,8 @@
       <c r="F178" s="4">
         <v>8453557083</v>
       </c>
-      <c r="G178" s="5">
-        <v>41056</v>
+      <c r="G178" s="5" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5713,8 +6274,8 @@
       <c r="F179" s="4">
         <v>5453547933</v>
       </c>
-      <c r="G179" s="5">
-        <v>41000</v>
+      <c r="G179" s="5" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5736,8 +6297,8 @@
       <c r="F180" s="4">
         <v>9239375721</v>
       </c>
-      <c r="G180" s="5">
-        <v>41132</v>
+      <c r="G180" s="5" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -5759,8 +6320,8 @@
       <c r="F181" s="4">
         <v>4568638094</v>
       </c>
-      <c r="G181" s="5">
-        <v>41133</v>
+      <c r="G181" s="5" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5782,8 +6343,8 @@
       <c r="F182" s="4">
         <v>7869628304</v>
       </c>
-      <c r="G182" s="5">
-        <v>40843</v>
+      <c r="G182" s="5" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -5805,8 +6366,8 @@
       <c r="F183" s="4">
         <v>3622264120</v>
       </c>
-      <c r="G183" s="5">
-        <v>40843</v>
+      <c r="G183" s="5" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5828,8 +6389,8 @@
       <c r="F184" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G184" s="5">
-        <v>41435</v>
+      <c r="G184" s="5" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5851,8 +6412,8 @@
       <c r="F185" s="4">
         <v>6630345001</v>
       </c>
-      <c r="G185" s="5">
-        <v>41009</v>
+      <c r="G185" s="5" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5874,8 +6435,8 @@
       <c r="F186" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G186" s="5">
-        <v>41180</v>
+      <c r="G186" s="5" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -5897,8 +6458,8 @@
       <c r="F187" s="4">
         <v>5665608494</v>
       </c>
-      <c r="G187" s="5">
-        <v>40933</v>
+      <c r="G187" s="5" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5920,8 +6481,8 @@
       <c r="F188" s="4">
         <v>3719</v>
       </c>
-      <c r="G188" s="5">
-        <v>41060</v>
+      <c r="G188" s="5" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5943,8 +6504,8 @@
       <c r="F189" s="4">
         <v>5820234360</v>
       </c>
-      <c r="G189" s="5">
-        <v>41126</v>
+      <c r="G189" s="5" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5966,8 +6527,8 @@
       <c r="F190" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="G190" s="5">
-        <v>41211</v>
+      <c r="G190" s="5" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -5989,8 +6550,8 @@
       <c r="F191" s="4">
         <v>5222215730</v>
       </c>
-      <c r="G191" s="5">
-        <v>41319</v>
+      <c r="G191" s="5" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -6012,8 +6573,8 @@
       <c r="F192" s="4">
         <v>6460679844</v>
       </c>
-      <c r="G192" s="5">
-        <v>41368</v>
+      <c r="G192" s="5" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -6035,8 +6596,8 @@
       <c r="F193" s="4">
         <v>7934387351</v>
       </c>
-      <c r="G193" s="5">
-        <v>41580</v>
+      <c r="G193" s="5" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -6058,8 +6619,8 @@
       <c r="F194" s="4">
         <v>9566658594</v>
       </c>
-      <c r="G194" s="5">
-        <v>41183</v>
+      <c r="G194" s="5" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -6081,8 +6642,8 @@
       <c r="F195" s="4">
         <v>8764649384</v>
       </c>
-      <c r="G195" s="5">
-        <v>41584</v>
+      <c r="G195" s="5" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -6104,8 +6665,8 @@
       <c r="F196" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="G196" s="5">
-        <v>41373</v>
+      <c r="G196" s="5" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -6127,8 +6688,8 @@
       <c r="F197" s="4">
         <v>1060669024</v>
       </c>
-      <c r="G197" s="5">
-        <v>41521</v>
+      <c r="G197" s="5" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -6150,8 +6711,8 @@
       <c r="F198" s="4">
         <v>8843445182</v>
       </c>
-      <c r="G198" s="5">
-        <v>40800</v>
+      <c r="G198" s="5" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -6173,8 +6734,8 @@
       <c r="F199" s="4">
         <v>9734375451</v>
       </c>
-      <c r="G199" s="5">
-        <v>40856</v>
+      <c r="G199" s="5" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -6196,8 +6757,8 @@
       <c r="F200" s="4">
         <v>5260668514</v>
       </c>
-      <c r="G200" s="5">
-        <v>40948</v>
+      <c r="G200" s="5" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -6219,8 +6780,8 @@
       <c r="F201" s="4">
         <v>6368647854</v>
       </c>
-      <c r="G201" s="5">
-        <v>40567</v>
+      <c r="G201" s="5" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -6242,8 +6803,8 @@
       <c r="F202" s="4">
         <v>4258517263</v>
       </c>
-      <c r="G202" s="5">
-        <v>41084</v>
+      <c r="G202" s="5" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -6265,8 +6826,8 @@
       <c r="F203" s="4">
         <v>6839304491</v>
       </c>
-      <c r="G203" s="5">
-        <v>40787</v>
+      <c r="G203" s="5" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6288,8 +6849,8 @@
       <c r="F204" s="4">
         <v>9945417992</v>
       </c>
-      <c r="G204" s="5">
-        <v>41620</v>
+      <c r="G204" s="5" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>